<commit_message>
Formatear datos y verificar
</commit_message>
<xml_diff>
--- a/PNuevoIngreso.xlsx
+++ b/PNuevoIngreso.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Archivos_mbarragan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Archivos_jtenorio\Documentos\Programacion\Automatizar\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -179,9 +179,6 @@
     <t>LIMA</t>
   </si>
   <si>
-    <t>AUXILIAR POST-VENTA</t>
-  </si>
-  <si>
     <t>LauBelloLima@gmail.com</t>
   </si>
   <si>
@@ -267,12 +264,15 @@
   </si>
   <si>
     <t>celisvictor839@gmail.com</t>
+  </si>
+  <si>
+    <t>AUXILIAR EN POST-VENTA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -629,8 +629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -893,7 +893,7 @@
         <v>50</v>
       </c>
       <c r="E10" t="s">
-        <v>51</v>
+        <v>80</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>42</v>
@@ -902,7 +902,7 @@
         <v>45688</v>
       </c>
       <c r="H10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -910,13 +910,13 @@
         <v>499</v>
       </c>
       <c r="B11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" t="s">
         <v>53</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>54</v>
-      </c>
-      <c r="D11" t="s">
-        <v>55</v>
       </c>
       <c r="E11" t="s">
         <v>41</v>
@@ -928,7 +928,7 @@
         <v>45692</v>
       </c>
       <c r="H11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -936,13 +936,13 @@
         <v>500</v>
       </c>
       <c r="B12" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" t="s">
         <v>57</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>58</v>
-      </c>
-      <c r="D12" t="s">
-        <v>59</v>
       </c>
       <c r="E12" t="s">
         <v>41</v>
@@ -954,7 +954,7 @@
         <v>45692</v>
       </c>
       <c r="H12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -962,13 +962,13 @@
         <v>501</v>
       </c>
       <c r="B13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" t="s">
         <v>61</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>62</v>
-      </c>
-      <c r="D13" t="s">
-        <v>63</v>
       </c>
       <c r="E13" t="s">
         <v>41</v>
@@ -980,7 +980,7 @@
         <v>45692</v>
       </c>
       <c r="H13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -988,13 +988,13 @@
         <v>502</v>
       </c>
       <c r="B14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" t="s">
         <v>65</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>66</v>
-      </c>
-      <c r="D14" t="s">
-        <v>67</v>
       </c>
       <c r="E14" t="s">
         <v>41</v>
@@ -1006,15 +1006,15 @@
         <v>45692</v>
       </c>
       <c r="H14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" t="s">
         <v>69</v>
-      </c>
-      <c r="B15" t="s">
-        <v>70</v>
       </c>
       <c r="C15" t="s">
         <v>36</v>
@@ -1032,21 +1032,21 @@
         <v>45692</v>
       </c>
       <c r="H15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B16" t="s">
         <v>72</v>
-      </c>
-      <c r="B16" t="s">
-        <v>73</v>
       </c>
       <c r="C16" t="s">
         <v>17</v>
       </c>
       <c r="D16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E16" t="s">
         <v>12</v>
@@ -1058,21 +1058,21 @@
         <v>45692</v>
       </c>
       <c r="H16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17" t="s">
         <v>76</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>77</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>78</v>
-      </c>
-      <c r="D17" t="s">
-        <v>79</v>
       </c>
       <c r="E17" t="s">
         <v>12</v>
@@ -1084,7 +1084,7 @@
         <v>45692</v>
       </c>
       <c r="H17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Generacion de formato para SQL
</commit_message>
<xml_diff>
--- a/PNuevoIngreso.xlsx
+++ b/PNuevoIngreso.xlsx
@@ -266,7 +266,7 @@
     <t>celisvictor839@gmail.com</t>
   </si>
   <si>
-    <t>AUXILIAR EN POST-VENTA</t>
+    <t>AUXILIAR POST-VENTA</t>
   </si>
 </sst>
 </file>
@@ -630,7 +630,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Cambios en la estructura del proyecto
</commit_message>
<xml_diff>
--- a/PNuevoIngreso.xlsx
+++ b/PNuevoIngreso.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Archivos_mbarragan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Archivos_jtenorio\OneDrive - TAURUS - ESPAÑA\Documentos\Programacion\Automatizar\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D75FE3BD-82DB-49F1-A1CC-4688B27FA1DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="2505" yWindow="795" windowWidth="15375" windowHeight="7785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
   <si>
     <t>NO EMP</t>
   </si>
@@ -50,13 +51,13 @@
     <t>E-MAIL</t>
   </si>
   <si>
-    <t>EMELIO</t>
-  </si>
-  <si>
-    <t>REYES</t>
-  </si>
-  <si>
-    <t>FLORES</t>
+    <t>ALBERTO ISABEL</t>
+  </si>
+  <si>
+    <t>CHAVEZ</t>
+  </si>
+  <si>
+    <t>HERNANDEZ</t>
   </si>
   <si>
     <t>ENSAMBLADOR</t>
@@ -65,118 +66,79 @@
     <t>BANCOR</t>
   </si>
   <si>
-    <t>Reyesemelio58@gmail.com</t>
-  </si>
-  <si>
-    <t>LORENA</t>
-  </si>
-  <si>
-    <t>CORTE</t>
-  </si>
-  <si>
-    <t>PEREZ</t>
-  </si>
-  <si>
-    <t>lcorteperez@gmail.com</t>
-  </si>
-  <si>
-    <t>VIVIANA</t>
-  </si>
-  <si>
-    <t>VAZQUEZ</t>
+    <t>albertochavez2404@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BIANCA JANET </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AZTATZI </t>
   </si>
   <si>
     <t>CUAPIO</t>
   </si>
   <si>
-    <t>vazquezcuapiov@gmail.com</t>
-  </si>
-  <si>
-    <t>MARIA DEL CARMEN</t>
-  </si>
-  <si>
-    <t>ORTEGA</t>
-  </si>
-  <si>
-    <t>ZAMBRANO</t>
-  </si>
-  <si>
-    <t>ortegazambranocarmen@gmail.com</t>
-  </si>
-  <si>
-    <t>GUSTAVO</t>
-  </si>
-  <si>
-    <t>GUERRERO</t>
-  </si>
-  <si>
-    <t>LUNA</t>
-  </si>
-  <si>
-    <t>guerrerogu485@gmail.com</t>
-  </si>
-  <si>
-    <t>YEIMI</t>
-  </si>
-  <si>
-    <t>RODRIGUEZ</t>
-  </si>
-  <si>
-    <t>ZEMPOALTECA</t>
-  </si>
-  <si>
-    <t>yeimirodriguezzempoalteca4538@gmail.com</t>
-  </si>
-  <si>
-    <t>LUCERO</t>
-  </si>
-  <si>
-    <t>MUÑOZ</t>
-  </si>
-  <si>
-    <t>munozlucero00@gmail.com</t>
-  </si>
-  <si>
-    <t>LUIS FERNANDO</t>
-  </si>
-  <si>
-    <t>SALDAÑA</t>
-  </si>
-  <si>
-    <t>CORONA</t>
-  </si>
-  <si>
-    <t>lfsc4019@gmail.com</t>
-  </si>
-  <si>
-    <t>NORBERTO</t>
-  </si>
-  <si>
-    <t>JIMENEZ</t>
-  </si>
-  <si>
-    <t>ROJAS</t>
-  </si>
-  <si>
-    <t>rjimenezr558@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LINDA PATRICIA </t>
-  </si>
-  <si>
-    <t>OREA</t>
-  </si>
-  <si>
-    <t>HERNANDEZ</t>
-  </si>
-  <si>
-    <t>oreahernandezlindapatricia@gmail.com</t>
+    <t>charlyfany@gmail.com</t>
+  </si>
+  <si>
+    <t>LEONARDO</t>
+  </si>
+  <si>
+    <t>SANCHEZ</t>
+  </si>
+  <si>
+    <t>Leocuapio900@gmail.com</t>
+  </si>
+  <si>
+    <t>YAZMIN LUCERO</t>
+  </si>
+  <si>
+    <t>PEÑA</t>
+  </si>
+  <si>
+    <t>COCOLETZI</t>
+  </si>
+  <si>
+    <t>yazlcrcc@gmail.com</t>
+  </si>
+  <si>
+    <t>SANDY</t>
+  </si>
+  <si>
+    <t>TECUAPACHO</t>
+  </si>
+  <si>
+    <t>ATONAL</t>
+  </si>
+  <si>
+    <t>atonaldayana@gmail.com</t>
+  </si>
+  <si>
+    <t>992L</t>
+  </si>
+  <si>
+    <t>OSCAR</t>
+  </si>
+  <si>
+    <t>GUARNEROS</t>
+  </si>
+  <si>
+    <t>BONILLA</t>
+  </si>
+  <si>
+    <t>LOGYM</t>
+  </si>
+  <si>
+    <t>oskrgubo3@gmail.com</t>
+  </si>
+  <si>
+    <t>SMED 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -211,14 +173,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -226,17 +188,17 @@
   </cellStyles>
   <dxfs count="4">
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -252,17 +214,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:H11" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:H11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla1" displayName="Tabla1" ref="A1:H7" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="A1:H7" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="NO EMP" dataDxfId="3"/>
-    <tableColumn id="2" name="NOMBRE"/>
-    <tableColumn id="3" name="APELLIDO PATERNO"/>
-    <tableColumn id="4" name="APELLIDO MATERNO"/>
-    <tableColumn id="5" name="PUESTO"/>
-    <tableColumn id="6" name="EMPRESA" dataDxfId="2"/>
-    <tableColumn id="7" name="FECHA DE ANTIGÜEDAD" dataDxfId="1"/>
-    <tableColumn id="8" name="E-MAIL"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="NO EMP" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="NOMBRE"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="APELLIDO PATERNO"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="APELLIDO MATERNO"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="PUESTO"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="EMPRESA" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="FECHA DE ANTIGÜEDAD" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="E-MAIL"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -530,54 +492,54 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.5703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="41.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="28.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:8" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>503</v>
+        <v>550</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -594,8 +556,8 @@
       <c r="F2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="2">
-        <v>45698</v>
+      <c r="G2" s="4">
+        <v>45769</v>
       </c>
       <c r="H2" t="s">
         <v>13</v>
@@ -603,7 +565,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>504</v>
+        <v>551</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
@@ -620,8 +582,8 @@
       <c r="F3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="2">
-        <v>45698</v>
+      <c r="G3" s="4">
+        <v>45769</v>
       </c>
       <c r="H3" t="s">
         <v>17</v>
@@ -629,16 +591,16 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>505</v>
+        <v>552</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
       </c>
       <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
         <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>20</v>
       </c>
       <c r="E4" t="s">
         <v>11</v>
@@ -646,25 +608,25 @@
       <c r="F4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="2">
-        <v>45698</v>
+      <c r="G4" s="4">
+        <v>45769</v>
       </c>
       <c r="H4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>506</v>
+        <v>553</v>
       </c>
       <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
         <v>22</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>23</v>
-      </c>
-      <c r="D5" t="s">
-        <v>24</v>
       </c>
       <c r="E5" t="s">
         <v>11</v>
@@ -672,25 +634,25 @@
       <c r="F5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="2">
-        <v>45698</v>
+      <c r="G5" s="4">
+        <v>45769</v>
       </c>
       <c r="H5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>507</v>
+        <v>554</v>
       </c>
       <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
         <v>26</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>27</v>
-      </c>
-      <c r="D6" t="s">
-        <v>28</v>
       </c>
       <c r="E6" t="s">
         <v>11</v>
@@ -698,16 +660,16 @@
       <c r="F6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="2">
-        <v>45698</v>
+      <c r="G6" s="4">
+        <v>45769</v>
       </c>
       <c r="H6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>508</v>
+      <c r="A7" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="B7" t="s">
         <v>30</v>
@@ -719,120 +681,16 @@
         <v>32</v>
       </c>
       <c r="E7" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="2">
-        <v>45698</v>
+        <v>33</v>
+      </c>
+      <c r="G7" s="4">
+        <v>45769</v>
       </c>
       <c r="H7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>509</v>
-      </c>
-      <c r="B8" t="s">
         <v>34</v>
-      </c>
-      <c r="C8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" s="2">
-        <v>45698</v>
-      </c>
-      <c r="H8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>510</v>
-      </c>
-      <c r="B9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" t="s">
-        <v>39</v>
-      </c>
-      <c r="E9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" s="2">
-        <v>45698</v>
-      </c>
-      <c r="H9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>511</v>
-      </c>
-      <c r="B10" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" s="2">
-        <v>45698</v>
-      </c>
-      <c r="H10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>512</v>
-      </c>
-      <c r="B11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" t="s">
-        <v>46</v>
-      </c>
-      <c r="D11" t="s">
-        <v>47</v>
-      </c>
-      <c r="E11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" s="2">
-        <v>45698</v>
-      </c>
-      <c r="H11" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>